<commit_message>
updated metadata files and organized assets folder, updated test confs
</commit_message>
<xml_diff>
--- a/assets/custom_meta_fields/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/custom_meta_fields/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankushgupta/Documents/tostadas/assets/custom_meta_fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/custom_meta_fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C29379-ACB1-7D44-B89A-1789603997D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E972A660-802A-274C-9488-AB2F3BE8EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPXV_Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="440">
   <si>
     <t>Strategy</t>
   </si>
@@ -1324,6 +1324,27 @@
   </si>
   <si>
     <t>TX0001_7.fasta</t>
+  </si>
+  <si>
+    <t>FL0004.fasta</t>
+  </si>
+  <si>
+    <t>IL0005.fasta</t>
+  </si>
+  <si>
+    <t>NY0006.fasta</t>
+  </si>
+  <si>
+    <t>NY0007.fasta</t>
+  </si>
+  <si>
+    <t>TX0001.fasta</t>
+  </si>
+  <si>
+    <t>FL0015.fasta</t>
+  </si>
+  <si>
+    <t>OH0002.fasta</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1439,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1478,6 +1499,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1569,7 +1596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1706,6 +1733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2011,992 +2039,1016 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AP46"/>
+  <dimension ref="A1:AQ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AP10" sqref="AP10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="20" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="38" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="41" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="39" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="13.5" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="T1" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="W1" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="X1" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="AE1" s="36" t="s">
+      <c r="AF1" s="36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="48" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>373</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>374</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M2" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="N2" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="O2" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="P2" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="Q2" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="R2" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="S2" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="S2" s="37" t="s">
+      <c r="T2" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="U2" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="V2" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="W2" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="X2" s="37" t="s">
         <v>288</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="Y2" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="Z2" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="AA2" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="AA2" s="20" t="s">
+      <c r="AB2" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AC2" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="AC2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="AD2" s="20" t="s">
+      <c r="AE2" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="AE2" s="37" t="s">
+      <c r="AF2" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AG2" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="AK2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AN2" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="AN2" s="21" t="s">
+      <c r="AO2" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="AO2" s="21" t="s">
+      <c r="AP2" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="AP2" s="45" t="s">
+      <c r="AQ2" s="45" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B3" t="s">
         <v>378</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>379</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>380</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>379</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>381</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>350</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>307</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>262</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>382</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>383</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="S3" t="s">
+      <c r="P3" s="36"/>
+      <c r="T3" t="s">
         <v>384</v>
       </c>
-      <c r="U3" s="14">
+      <c r="V3" s="14">
         <v>247</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>385</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>216</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>4</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>73</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>85</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>310</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>386</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>387</v>
       </c>
-      <c r="AE3" s="36"/>
-      <c r="AM3" s="14" t="s">
+      <c r="AF3" s="36"/>
+      <c r="AN3" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="AN3" s="17">
+      <c r="AO3" s="17">
         <v>50</v>
       </c>
-      <c r="AO3" s="14">
+      <c r="AP3" s="14">
         <v>1</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B4" t="s">
         <v>389</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>390</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>391</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>390</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>381</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>350</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>307</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>392</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>393</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="S4" t="s">
+      <c r="P4" s="36"/>
+      <c r="T4" t="s">
         <v>394</v>
       </c>
-      <c r="U4" s="14">
+      <c r="V4" s="14">
         <v>40</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>395</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>216</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>4</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>73</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>310</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>396</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>397</v>
       </c>
-      <c r="AE4" s="36"/>
-      <c r="AM4" s="14">
+      <c r="AF4" s="36"/>
+      <c r="AN4" s="14">
         <v>5</v>
       </c>
-      <c r="AN4" s="16">
+      <c r="AO4" s="16">
         <v>3.5</v>
       </c>
-      <c r="AO4" s="14">
+      <c r="AP4" s="14">
         <v>0</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B5" t="s">
         <v>398</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>399</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>400</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>399</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>381</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>350</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>307</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>401</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>402</v>
       </c>
-      <c r="O5" s="36"/>
-      <c r="S5" t="s">
+      <c r="P5" s="36"/>
+      <c r="T5" t="s">
         <v>403</v>
       </c>
-      <c r="U5" s="14">
+      <c r="V5" s="14">
         <v>121</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>404</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>216</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>73</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>85</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>310</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>405</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>406</v>
       </c>
-      <c r="AE5" s="36"/>
-      <c r="AM5" s="14">
+      <c r="AF5" s="36"/>
+      <c r="AN5" s="14">
         <v>8</v>
       </c>
-      <c r="AN5" s="14">
+      <c r="AO5" s="14">
         <v>3</v>
       </c>
-      <c r="AO5" s="14">
+      <c r="AP5" s="14">
         <v>0</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B6" t="s">
         <v>407</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>408</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>400</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>408</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>381</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>350</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>307</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>401</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>382</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>409</v>
       </c>
-      <c r="O6" s="36"/>
-      <c r="S6" t="s">
+      <c r="P6" s="36"/>
+      <c r="T6" t="s">
         <v>410</v>
       </c>
-      <c r="U6" s="14">
+      <c r="V6" s="14">
         <v>72</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>411</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>216</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>4</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>73</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>85</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>310</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>412</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>413</v>
       </c>
-      <c r="AE6" s="36"/>
-      <c r="AM6" s="14">
+      <c r="AF6" s="36"/>
+      <c r="AN6" s="14">
         <v>4</v>
       </c>
-      <c r="AN6" s="16">
+      <c r="AO6" s="16">
         <v>3.2</v>
       </c>
-      <c r="AO6" s="14">
+      <c r="AP6" s="14">
         <v>1</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B7" t="s">
         <v>414</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>415</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>416</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>415</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>381</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>350</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>307</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>417</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>382</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>383</v>
       </c>
-      <c r="O7" s="36"/>
-      <c r="S7" t="s">
+      <c r="P7" s="36"/>
+      <c r="T7" t="s">
         <v>418</v>
       </c>
-      <c r="U7" s="14">
+      <c r="V7" s="14">
         <v>73</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>419</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>216</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>4</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>73</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>85</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>310</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>420</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>421</v>
       </c>
-      <c r="AE7" s="36"/>
-      <c r="AM7" s="17" t="s">
+      <c r="AF7" s="36"/>
+      <c r="AN7" s="17" t="s">
         <v>422</v>
       </c>
-      <c r="AN7" s="16">
+      <c r="AO7" s="16">
         <v>1.5</v>
       </c>
-      <c r="AO7" s="14">
+      <c r="AP7" s="14">
         <v>0</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>438</v>
+      </c>
+      <c r="B8" t="s">
         <v>423</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>415</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>416</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>415</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>381</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>350</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>307</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>417</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>382</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>383</v>
       </c>
-      <c r="O8" s="36"/>
-      <c r="S8" t="s">
+      <c r="P8" s="36"/>
+      <c r="T8" t="s">
         <v>418</v>
       </c>
-      <c r="U8" s="14">
+      <c r="V8" s="14">
         <v>73</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>419</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>216</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>4</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>73</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>85</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>310</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>420</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>421</v>
       </c>
-      <c r="AE8" s="36"/>
-      <c r="AM8" s="14">
+      <c r="AF8" s="36"/>
+      <c r="AN8" s="14">
         <v>3</v>
-      </c>
-      <c r="AN8" s="14">
-        <v>1</v>
       </c>
       <c r="AO8" s="14">
         <v>1</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AP8" s="14">
+        <v>1</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="9" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" t="s">
         <v>424</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>415</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>416</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>415</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>381</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>350</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>307</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>417</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>382</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>383</v>
       </c>
-      <c r="O9" s="36"/>
-      <c r="S9" t="s">
+      <c r="P9" s="36"/>
+      <c r="T9" t="s">
         <v>418</v>
       </c>
-      <c r="U9" s="14">
+      <c r="V9" s="14">
         <v>73</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>419</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>216</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>4</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>73</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>85</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>310</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>420</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>421</v>
       </c>
-      <c r="AE9" s="36"/>
-      <c r="AM9" s="17" t="s">
+      <c r="AF9" s="36"/>
+      <c r="AN9" s="17" t="s">
         <v>422</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="S10" s="36"/>
-      <c r="V10" s="36"/>
+    <row r="10" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="T10" s="36"/>
       <c r="W10" s="36"/>
-      <c r="AE10" s="36"/>
-    </row>
-    <row r="11" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="V11" s="36"/>
+      <c r="X10" s="36"/>
+      <c r="AF10" s="36"/>
+    </row>
+    <row r="11" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="T11" s="36"/>
       <c r="W11" s="36"/>
-      <c r="AE11" s="36"/>
-    </row>
-    <row r="12" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="V12" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="AF11" s="36"/>
+    </row>
+    <row r="12" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="T12" s="36"/>
       <c r="W12" s="36"/>
-      <c r="AE12" s="36"/>
-    </row>
-    <row r="13" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="V13" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="AF12" s="36"/>
+    </row>
+    <row r="13" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="T13" s="36"/>
       <c r="W13" s="36"/>
-      <c r="AE13" s="36"/>
-    </row>
-    <row r="14" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="V14" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="AF13" s="36"/>
+    </row>
+    <row r="14" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="T14" s="36"/>
       <c r="W14" s="36"/>
-      <c r="AE14" s="36"/>
-    </row>
-    <row r="15" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="V15" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="AF14" s="36"/>
+    </row>
+    <row r="15" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="T15" s="36"/>
       <c r="W15" s="36"/>
-      <c r="AE15" s="36"/>
-    </row>
-    <row r="16" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="V16" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="AF15" s="36"/>
+    </row>
+    <row r="16" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="T16" s="36"/>
       <c r="W16" s="36"/>
-      <c r="AE16" s="36"/>
-    </row>
-    <row r="17" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="V17" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="AF16" s="36"/>
+    </row>
+    <row r="17" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="T17" s="36"/>
       <c r="W17" s="36"/>
-      <c r="AE17" s="36"/>
-    </row>
-    <row r="18" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="V18" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="AF17" s="36"/>
+    </row>
+    <row r="18" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="T18" s="36"/>
       <c r="W18" s="36"/>
-      <c r="AE18" s="36"/>
-    </row>
-    <row r="19" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="V19" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="AF18" s="36"/>
+    </row>
+    <row r="19" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="T19" s="36"/>
       <c r="W19" s="36"/>
-      <c r="AE19" s="36"/>
-    </row>
-    <row r="20" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="V20" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="AF19" s="36"/>
+    </row>
+    <row r="20" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="T20" s="36"/>
       <c r="W20" s="36"/>
-      <c r="AE20" s="36"/>
-    </row>
-    <row r="21" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="V21" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="AF20" s="36"/>
+    </row>
+    <row r="21" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="T21" s="36"/>
       <c r="W21" s="36"/>
-      <c r="AE21" s="36"/>
-    </row>
-    <row r="22" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="V22" s="36"/>
+      <c r="X21" s="36"/>
+      <c r="AF21" s="36"/>
+    </row>
+    <row r="22" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="T22" s="36"/>
       <c r="W22" s="36"/>
-      <c r="AE22" s="36"/>
-    </row>
-    <row r="23" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="V23" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="AF22" s="36"/>
+    </row>
+    <row r="23" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="T23" s="36"/>
       <c r="W23" s="36"/>
-      <c r="AE23" s="36"/>
-    </row>
-    <row r="24" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="V24" s="36"/>
+      <c r="X23" s="36"/>
+      <c r="AF23" s="36"/>
+    </row>
+    <row r="24" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="T24" s="36"/>
       <c r="W24" s="36"/>
-      <c r="AE24" s="36"/>
-    </row>
-    <row r="25" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="V25" s="36"/>
+      <c r="X24" s="36"/>
+      <c r="AF24" s="36"/>
+    </row>
+    <row r="25" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="T25" s="36"/>
       <c r="W25" s="36"/>
-      <c r="AE25" s="36"/>
-    </row>
-    <row r="26" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="V26" s="36"/>
+      <c r="X25" s="36"/>
+      <c r="AF25" s="36"/>
+    </row>
+    <row r="26" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="T26" s="36"/>
       <c r="W26" s="36"/>
-      <c r="AE26" s="36"/>
-    </row>
-    <row r="27" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D27" s="36"/>
-      <c r="O27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="V27" s="36"/>
+      <c r="X26" s="36"/>
+      <c r="AF26" s="36"/>
+    </row>
+    <row r="27" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="T27" s="36"/>
       <c r="W27" s="36"/>
-      <c r="AE27" s="36"/>
-    </row>
-    <row r="28" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D28" s="36"/>
-      <c r="O28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="V28" s="36"/>
+      <c r="X27" s="36"/>
+      <c r="AF27" s="36"/>
+    </row>
+    <row r="28" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="T28" s="36"/>
       <c r="W28" s="36"/>
-      <c r="AE28" s="36"/>
-    </row>
-    <row r="29" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D29" s="36"/>
-      <c r="O29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="V29" s="36"/>
+      <c r="X28" s="36"/>
+      <c r="AF28" s="36"/>
+    </row>
+    <row r="29" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="T29" s="36"/>
       <c r="W29" s="36"/>
-      <c r="AE29" s="36"/>
-    </row>
-    <row r="30" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D30" s="36"/>
-      <c r="O30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="V30" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="AF29" s="36"/>
+    </row>
+    <row r="30" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="T30" s="36"/>
       <c r="W30" s="36"/>
-      <c r="AE30" s="36"/>
-    </row>
-    <row r="31" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="V31" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="AF30" s="36"/>
+    </row>
+    <row r="31" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="T31" s="36"/>
       <c r="W31" s="36"/>
-      <c r="AE31" s="36"/>
-    </row>
-    <row r="32" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="V32" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="AF31" s="36"/>
+    </row>
+    <row r="32" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="T32" s="36"/>
       <c r="W32" s="36"/>
-      <c r="AE32" s="36"/>
-    </row>
-    <row r="33" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="V33" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="AF32" s="36"/>
+    </row>
+    <row r="33" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="T33" s="36"/>
       <c r="W33" s="36"/>
-      <c r="AE33" s="36"/>
-    </row>
-    <row r="34" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D34" s="36"/>
-      <c r="O34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="V34" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="AF33" s="36"/>
+    </row>
+    <row r="34" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="T34" s="36"/>
       <c r="W34" s="36"/>
-      <c r="AE34" s="36"/>
-    </row>
-    <row r="35" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D35" s="36"/>
-      <c r="O35" s="36"/>
-      <c r="S35" s="36"/>
-      <c r="V35" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="AF34" s="36"/>
+    </row>
+    <row r="35" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="36"/>
+      <c r="P35" s="36"/>
+      <c r="T35" s="36"/>
       <c r="W35" s="36"/>
-      <c r="AE35" s="36"/>
-    </row>
-    <row r="36" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D36" s="36"/>
-      <c r="O36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="V36" s="36"/>
+      <c r="X35" s="36"/>
+      <c r="AF35" s="36"/>
+    </row>
+    <row r="36" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="T36" s="36"/>
       <c r="W36" s="36"/>
-      <c r="AE36" s="36"/>
-    </row>
-    <row r="37" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D37" s="36"/>
-      <c r="O37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="V37" s="36"/>
+      <c r="X36" s="36"/>
+      <c r="AF36" s="36"/>
+    </row>
+    <row r="37" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E37" s="36"/>
+      <c r="P37" s="36"/>
+      <c r="T37" s="36"/>
       <c r="W37" s="36"/>
-      <c r="AE37" s="36"/>
-    </row>
-    <row r="38" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D38" s="36"/>
-      <c r="O38" s="36"/>
-      <c r="S38" s="36"/>
-      <c r="V38" s="36"/>
+      <c r="X37" s="36"/>
+      <c r="AF37" s="36"/>
+    </row>
+    <row r="38" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="36"/>
+      <c r="P38" s="36"/>
+      <c r="T38" s="36"/>
       <c r="W38" s="36"/>
-      <c r="AE38" s="36"/>
-    </row>
-    <row r="39" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="V39" s="36"/>
+      <c r="X38" s="36"/>
+      <c r="AF38" s="36"/>
+    </row>
+    <row r="39" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="T39" s="36"/>
       <c r="W39" s="36"/>
-      <c r="AE39" s="36"/>
-    </row>
-    <row r="40" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="V40" s="36"/>
+      <c r="X39" s="36"/>
+      <c r="AF39" s="36"/>
+    </row>
+    <row r="40" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="T40" s="36"/>
       <c r="W40" s="36"/>
-      <c r="AE40" s="36"/>
-    </row>
-    <row r="41" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="S41" s="36"/>
-      <c r="V41" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="AF40" s="36"/>
+    </row>
+    <row r="41" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="T41" s="36"/>
       <c r="W41" s="36"/>
-      <c r="AE41" s="36"/>
-    </row>
-    <row r="42" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D42" s="36"/>
-      <c r="O42" s="36"/>
-      <c r="S42" s="36"/>
-      <c r="V42" s="36"/>
+      <c r="X41" s="36"/>
+      <c r="AF41" s="36"/>
+    </row>
+    <row r="42" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E42" s="36"/>
+      <c r="P42" s="36"/>
+      <c r="T42" s="36"/>
       <c r="W42" s="36"/>
-      <c r="AE42" s="36"/>
-    </row>
-    <row r="43" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D43" s="36"/>
-      <c r="O43" s="36"/>
-      <c r="S43" s="36"/>
-      <c r="V43" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="AF42" s="36"/>
+    </row>
+    <row r="43" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="T43" s="36"/>
       <c r="W43" s="36"/>
-      <c r="AE43" s="36"/>
-    </row>
-    <row r="44" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="36"/>
-      <c r="O44" s="36"/>
-      <c r="S44" s="36"/>
-      <c r="V44" s="36"/>
+      <c r="X43" s="36"/>
+      <c r="AF43" s="36"/>
+    </row>
+    <row r="44" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E44" s="36"/>
+      <c r="P44" s="36"/>
+      <c r="T44" s="36"/>
       <c r="W44" s="36"/>
-      <c r="AE44" s="36"/>
-    </row>
-    <row r="45" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="36"/>
-      <c r="O45" s="36"/>
-      <c r="S45" s="36"/>
-      <c r="V45" s="36"/>
+      <c r="X44" s="36"/>
+      <c r="AF44" s="36"/>
+    </row>
+    <row r="45" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E45" s="36"/>
+      <c r="P45" s="36"/>
+      <c r="T45" s="36"/>
       <c r="W45" s="36"/>
-      <c r="AE45" s="36"/>
-    </row>
-    <row r="46" spans="4:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="36"/>
-      <c r="O46" s="36"/>
-      <c r="S46" s="36"/>
-      <c r="V46" s="36"/>
+      <c r="X45" s="36"/>
+      <c r="AF45" s="36"/>
+    </row>
+    <row r="46" spans="5:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E46" s="36"/>
+      <c r="P46" s="36"/>
+      <c r="T46" s="36"/>
       <c r="W46" s="36"/>
-      <c r="AE46" s="36"/>
+      <c r="X46" s="36"/>
+      <c r="AF46" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6694,61 +6746,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6757,6 +6754,61 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added host to custom metafile
</commit_message>
<xml_diff>
--- a/assets/custom_meta_fields/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/custom_meta_fields/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/custom_meta_fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E972A660-802A-274C-9488-AB2F3BE8EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4A1489-3C8E-B94B-95B3-BDF06F2CED1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="441">
   <si>
     <t>Strategy</t>
   </si>
@@ -1345,6 +1345,9 @@
   </si>
   <si>
     <t>OH0002.fasta</t>
+  </si>
+  <si>
+    <t>human</t>
   </si>
 </sst>
 </file>
@@ -1727,13 +1730,13 @@
     <xf numFmtId="3" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2042,7 +2045,7 @@
   <dimension ref="A1:AQ46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2086,7 +2089,7 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>425</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -2229,6 +2232,9 @@
       <c r="E3" t="s">
         <v>379</v>
       </c>
+      <c r="G3" t="s">
+        <v>440</v>
+      </c>
       <c r="H3" t="s">
         <v>381</v>
       </c>
@@ -2308,6 +2314,9 @@
       <c r="E4" t="s">
         <v>390</v>
       </c>
+      <c r="G4" t="s">
+        <v>440</v>
+      </c>
       <c r="H4" t="s">
         <v>381</v>
       </c>
@@ -2384,6 +2393,9 @@
       <c r="E5" t="s">
         <v>399</v>
       </c>
+      <c r="G5" t="s">
+        <v>440</v>
+      </c>
       <c r="H5" t="s">
         <v>381</v>
       </c>
@@ -2460,6 +2472,9 @@
       <c r="E6" t="s">
         <v>408</v>
       </c>
+      <c r="G6" t="s">
+        <v>440</v>
+      </c>
       <c r="H6" t="s">
         <v>381</v>
       </c>
@@ -2539,6 +2554,9 @@
       <c r="E7" t="s">
         <v>415</v>
       </c>
+      <c r="G7" t="s">
+        <v>440</v>
+      </c>
       <c r="H7" t="s">
         <v>381</v>
       </c>
@@ -2618,6 +2636,9 @@
       <c r="E8" t="s">
         <v>415</v>
       </c>
+      <c r="G8" t="s">
+        <v>440</v>
+      </c>
       <c r="H8" t="s">
         <v>381</v>
       </c>
@@ -2696,6 +2717,9 @@
       </c>
       <c r="E9" t="s">
         <v>415</v>
+      </c>
+      <c r="G9" t="s">
+        <v>440</v>
       </c>
       <c r="H9" t="s">
         <v>381</v>
@@ -4885,8 +4909,8 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4900,10 +4924,10 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -4917,10 +4941,10 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4934,10 +4958,10 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -4951,10 +4975,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="46"/>
+      <c r="C5" s="47"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4968,10 +4992,10 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4985,10 +5009,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -5002,10 +5026,10 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -5019,10 +5043,10 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -5036,10 +5060,10 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -5053,10 +5077,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -5070,10 +5094,10 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5087,10 +5111,10 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -5104,10 +5128,10 @@
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -5121,10 +5145,10 @@
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="46"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -5138,10 +5162,10 @@
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="46"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -5155,10 +5179,10 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -5172,10 +5196,10 @@
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -5189,10 +5213,10 @@
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -5206,10 +5230,10 @@
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="46"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -5223,10 +5247,10 @@
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="46"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -5240,10 +5264,10 @@
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="46"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -5257,10 +5281,10 @@
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="46"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -5274,10 +5298,10 @@
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="46"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -5487,10 +5511,10 @@
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="46"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5502,8 +5526,8 @@
     </row>
     <row r="38" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5517,10 +5541,10 @@
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="47"/>
+      <c r="C39" s="48"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -5534,10 +5558,10 @@
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="46"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -5551,10 +5575,10 @@
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="46"/>
+      <c r="C41" s="47"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -5568,10 +5592,10 @@
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="46"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -5585,10 +5609,10 @@
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="46"/>
+      <c r="C43" s="47"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -5602,10 +5626,10 @@
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="46"/>
+      <c r="C44" s="47"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -5619,10 +5643,10 @@
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="46"/>
+      <c r="C45" s="47"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -5666,10 +5690,10 @@
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="46"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -5681,8 +5705,8 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -5696,10 +5720,10 @@
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="46"/>
+      <c r="C50" s="47"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -5713,10 +5737,10 @@
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="46"/>
+      <c r="C51" s="47"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -5730,10 +5754,10 @@
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="46"/>
+      <c r="C52" s="47"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -5747,10 +5771,10 @@
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="46" t="s">
+      <c r="B53" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="46"/>
+      <c r="C53" s="47"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -5764,10 +5788,10 @@
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="B54" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="46"/>
+      <c r="C54" s="47"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -5781,10 +5805,10 @@
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="46"/>
+      <c r="C55" s="47"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -5798,10 +5822,10 @@
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="46" t="s">
+      <c r="B56" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="46"/>
+      <c r="C56" s="47"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -5815,10 +5839,10 @@
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="46" t="s">
+      <c r="B57" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="46"/>
+      <c r="C57" s="47"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -5832,10 +5856,10 @@
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="46"/>
+      <c r="C58" s="47"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -5849,10 +5873,10 @@
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="46"/>
+      <c r="C59" s="47"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -5866,10 +5890,10 @@
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B60" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="46"/>
+      <c r="C60" s="47"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -5883,10 +5907,10 @@
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="46"/>
+      <c r="C61" s="47"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -5900,10 +5924,10 @@
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="46" t="s">
+      <c r="B62" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="46"/>
+      <c r="C62" s="47"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -5917,10 +5941,10 @@
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="46"/>
+      <c r="C63" s="47"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -5934,10 +5958,10 @@
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="46"/>
+      <c r="C64" s="47"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -5951,10 +5975,10 @@
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="46"/>
+      <c r="C65" s="47"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -5968,10 +5992,10 @@
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="46"/>
+      <c r="C66" s="47"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -5985,10 +6009,10 @@
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="46"/>
+      <c r="C67" s="47"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -6002,10 +6026,10 @@
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="46"/>
+      <c r="C68" s="47"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -6019,10 +6043,10 @@
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="C69" s="46"/>
+      <c r="C69" s="47"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -6036,10 +6060,10 @@
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="46" t="s">
+      <c r="B70" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="46"/>
+      <c r="C70" s="47"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -6053,10 +6077,10 @@
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="C71" s="46"/>
+      <c r="C71" s="47"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -6070,10 +6094,10 @@
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="46"/>
+      <c r="C72" s="47"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -6087,10 +6111,10 @@
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="46" t="s">
+      <c r="B73" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="46"/>
+      <c r="C73" s="47"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -6104,10 +6128,10 @@
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B74" s="46" t="s">
+      <c r="B74" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="46"/>
+      <c r="C74" s="47"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -6121,10 +6145,10 @@
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="46" t="s">
+      <c r="B75" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="46"/>
+      <c r="C75" s="47"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -6138,10 +6162,10 @@
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="C76" s="46"/>
+      <c r="C76" s="47"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -6155,10 +6179,10 @@
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="46" t="s">
+      <c r="B77" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="46"/>
+      <c r="C77" s="47"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -6746,6 +6770,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6754,61 +6833,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>